<commit_message>
Different Website Database (https://www.thespike.gg/player/t3xture/13470)
</commit_message>
<xml_diff>
--- a/Player_Data/Karon_Player_Data.xlsx
+++ b/Player_Data/Karon_Player_Data.xlsx
@@ -518,59 +518,59 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 75</t>
+          <t xml:space="preserve"> 77</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>193</v>
+        <v>213</v>
       </c>
       <c r="C2" t="n">
-        <v>0.99</v>
+        <v>1.01</v>
       </c>
       <c r="D2" t="n">
-        <v>175.6</v>
+        <v>178.6</v>
       </c>
       <c r="E2" t="n">
-        <v>0.91</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="F2" t="n">
-        <v>116.7</v>
+        <v>118.7</v>
       </c>
       <c r="G2" t="n">
-        <v>0.74</v>
+        <v>0.73</v>
       </c>
       <c r="H2" t="n">
-        <v>0.65</v>
+        <v>0.66</v>
       </c>
       <c r="I2" t="n">
         <v>0.39</v>
       </c>
       <c r="J2" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="K2" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="L2" t="n">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="M2" t="n">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="N2" t="n">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="O2" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="P2" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 17</t>
+          <t xml:space="preserve"> 15</t>
         </is>
       </c>
       <c r="B3" t="n">

</xml_diff>

<commit_message>
Spike-Database Didn't  work, alter original website to print player data per game map.
</commit_message>
<xml_diff>
--- a/Player_Data/Karon_Player_Data.xlsx
+++ b/Player_Data/Karon_Player_Data.xlsx
@@ -518,7 +518,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 77</t>
+          <t xml:space="preserve"> 67</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -570,29 +570,29 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 15</t>
+          <t xml:space="preserve"> 20</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="C3" t="n">
-        <v>1.18</v>
+        <v>1.11</v>
       </c>
       <c r="D3" t="n">
-        <v>224.5</v>
+        <v>204</v>
       </c>
       <c r="E3" t="n">
-        <v>1.22</v>
+        <v>1.06</v>
       </c>
       <c r="F3" t="n">
-        <v>132.6</v>
+        <v>125.6</v>
       </c>
       <c r="G3" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.79</v>
       </c>
       <c r="H3" t="n">
-        <v>0.83</v>
+        <v>0.73</v>
       </c>
       <c r="I3" t="n">
         <v>0.34</v>
@@ -601,74 +601,74 @@
         <v>0.09</v>
       </c>
       <c r="K3" t="n">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="L3" t="n">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="M3" t="n">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="N3" t="n">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="O3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 8</t>
+          <t xml:space="preserve"> 13</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="C4" t="n">
-        <v>0.87</v>
+        <v>1.07</v>
       </c>
       <c r="D4" t="n">
-        <v>136</v>
+        <v>163</v>
       </c>
       <c r="E4" t="n">
-        <v>0.65</v>
+        <v>0.84</v>
       </c>
       <c r="F4" t="n">
-        <v>100</v>
+        <v>110.7</v>
       </c>
       <c r="G4" t="n">
-        <v>0.67</v>
+        <v>0.73</v>
       </c>
       <c r="H4" t="n">
-        <v>0.46</v>
+        <v>0.54</v>
       </c>
       <c r="I4" t="n">
-        <v>0.25</v>
+        <v>0.44</v>
       </c>
       <c r="J4" t="n">
-        <v>0.17</v>
+        <v>0.15</v>
       </c>
       <c r="K4" t="n">
-        <v>0.13</v>
+        <v>0.08</v>
       </c>
       <c r="L4" t="n">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="M4" t="n">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="N4" t="n">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="O4" t="n">
+        <v>7</v>
+      </c>
+      <c r="P4" t="n">
         <v>4</v>
-      </c>
-      <c r="P4" t="n">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>